<commit_message>
PoC - workflow with hub+devices
</commit_message>
<xml_diff>
--- a/config/custom_components/damper/data structure.xlsx
+++ b/config/custom_components/damper/data structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\core\config\custom_components\damper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9510AD-2401-491B-9D6A-AA6BB8C79159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FBCE15-ECD1-434C-9C6A-BA847C178FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2081,11 +2081,22 @@
             </a:rPr>
             <a:t>async_create_entry(title=info["title"], data=user_input)</a:t>
           </a:r>
-          <a:endParaRPr lang="en-CH" sz="1100" b="1" baseline="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
+          <a:r>
+            <a:rPr lang="en-CH" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CH" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>&lt;- This triggers __init__.py</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -2120,11 +2131,46 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(gets called via __init__.py after config entry has been created, and after every restart of hassio)</a:t>
+          </a:r>
+          <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-CH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- safe instance of Hub to hass</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-CH" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>- safe device entries in hass:</a:t>
           </a:r>
         </a:p>
@@ -2136,7 +2182,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> - async_setup_entry: (gets called via __init__.py after config entry has been created, and after every restart of hassio)</a:t>
+            <a:t>   - async_setup_entry: </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2147,7 +2193,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>      - add every damper instance as a device: </a:t>
+            <a:t>        - add every damper instance as a device: </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2158,7 +2204,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>        async_add_devices( [Example Damper 1, Example Damper 2, ....])</a:t>
+            <a:t>          async_add_devices( [Example Damper 1, Example Damper 2, ....])</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2620,15 +2666,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>129989</xdr:colOff>
+      <xdr:colOff>129990</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>29138</xdr:rowOff>
+      <xdr:rowOff>29139</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>100852</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2643,8 +2689,64 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2012577" y="6315638"/>
-          <a:ext cx="7848599" cy="1382803"/>
+          <a:off x="2012578" y="6315639"/>
+          <a:ext cx="5573804" cy="497537"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>336176</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>103094</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>551330</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Arrow Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55F34A35-0A00-4AEA-8700-A4373D386EE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10096500" y="6961094"/>
+          <a:ext cx="1425389" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>

</xml_diff>

<commit_message>
Using "hass.config.path( ...)" to get path to Config folder
</commit_message>
<xml_diff>
--- a/config/custom_components/damper/data structure.xlsx
+++ b/config/custom_components/damper/data structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\core\config\custom_components\damper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FBCE15-ECD1-434C-9C6A-BA847C178FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27E248A-E28D-4B62-B92E-F901C1185B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1940,7 +1940,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>-</a:t>
@@ -1948,7 +1948,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t> ask user for com port, name</a:t>
@@ -1959,7 +1959,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- generate new hub instance with an empty array of damper instances</a:t>
@@ -1978,7 +1978,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- ask user for modbus address</a:t>
@@ -1989,7 +1989,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- add damper instance</a:t>
@@ -2000,7 +2000,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- repeat until user stops</a:t>
@@ -2019,10 +2019,10 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>- safe hub instance to a fle (pickle.py)</a:t>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- save hub instance to a file (pickle.py)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2057,7 +2057,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- safe integration config entry in hass:</a:t>
@@ -2068,7 +2068,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>  - </a:t>
@@ -2076,7 +2076,7 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100" b="1" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>async_create_entry(title=info["title"], data=user_input)</a:t>
@@ -2084,18 +2084,10 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" b="1" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CH" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>&lt;- This triggers __init__.py</a:t>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>    &lt;- This triggers __init__.py</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2133,7 +2125,7 @@
           <a:r>
             <a:rPr lang="de-DE" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>(gets called via __init__.py after config entry has been created, and after every restart of hassio)</a:t>
@@ -2141,14 +2133,14 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>:</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="1100" baseline="0">
             <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
           </a:endParaRPr>
         </a:p>
@@ -2157,7 +2149,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- safe instance of Hub to hass</a:t>
@@ -2168,7 +2160,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>- safe device entries in hass:</a:t>
@@ -2179,7 +2171,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>   - async_setup_entry: </a:t>
@@ -2190,7 +2182,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>        - add every damper instance as a device: </a:t>
@@ -2201,7 +2193,7 @@
           <a:r>
             <a:rPr lang="en-CH" sz="1100" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
             </a:rPr>
             <a:t>          async_add_devices( [Example Damper 1, Example Damper 2, ....])</a:t>
@@ -3044,7 +3036,7 @@
   <dimension ref="B1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>